<commit_message>
forral fighter hero & stat calcul
</commit_message>
<xml_diff>
--- a/modding resources/Stats_Calc.xlsx
+++ b/modding resources/Stats_Calc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFOLDER\IanLee\FOTR Submodding assests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFOLDER\IanLee\FOTR Submodding assests\FotR_Enhanced\modding resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F524A1-4454-4907-BC57-D5474224D9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334547C8-A7E5-4FBF-AB9A-998FE918115C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,7 +781,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="197">
   <si>
     <t>Unit</t>
   </si>
@@ -1369,6 +1369,10 @@
   </si>
   <si>
     <t>Template Venator Hero</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Umbaran Frigate</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1962,7 +1966,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2509,9 +2513,15 @@
       <c r="BJ4" s="5"/>
     </row>
     <row r="5" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1200</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>

</xml_diff>

<commit_message>
A6 done, unit test map configured
</commit_message>
<xml_diff>
--- a/modding resources/Stats_Calc.xlsx
+++ b/modding resources/Stats_Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFOLDER\IanLee\FOTR Submodding assests\FotR_Enhanced\modding resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F89B7F-5A20-46F6-A42F-2569CE9C2D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D946B4D5-EDA5-48C4-93C2-E9885FF9821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,7 +781,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="199">
   <si>
     <t>Unit</t>
   </si>
@@ -1380,6 +1380,10 @@
     <t>Pop</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>ArmourG_</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1722,6 +1726,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1745,9 +1752,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1974,7 +1978,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2003,91 +2007,91 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="61" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="63" t="s">
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="63" t="s">
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="58"/>
-      <c r="AE1" s="58"/>
-      <c r="AF1" s="57" t="s">
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="58"/>
-      <c r="AI1" s="58"/>
-      <c r="AJ1" s="58"/>
-      <c r="AK1" s="58"/>
-      <c r="AL1" s="57" t="s">
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="59"/>
+      <c r="AL1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="58"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="58"/>
-      <c r="AQ1" s="58"/>
-      <c r="AR1" s="57" t="s">
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="59"/>
+      <c r="AP1" s="59"/>
+      <c r="AQ1" s="59"/>
+      <c r="AR1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="58"/>
-      <c r="AV1" s="58"/>
-      <c r="AW1" s="58"/>
-      <c r="AX1" s="55" t="s">
+      <c r="AS1" s="59"/>
+      <c r="AT1" s="59"/>
+      <c r="AU1" s="59"/>
+      <c r="AV1" s="59"/>
+      <c r="AW1" s="59"/>
+      <c r="AX1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="AY1" s="56"/>
-      <c r="AZ1" s="56"/>
-      <c r="BA1" s="56"/>
-      <c r="BB1" s="56"/>
-      <c r="BC1" s="56"/>
-      <c r="BD1" s="56"/>
-      <c r="BE1" s="56"/>
-      <c r="BF1" s="56"/>
-      <c r="BG1" s="56"/>
-      <c r="BH1" s="57" t="s">
+      <c r="AY1" s="57"/>
+      <c r="AZ1" s="57"/>
+      <c r="BA1" s="57"/>
+      <c r="BB1" s="57"/>
+      <c r="BC1" s="57"/>
+      <c r="BD1" s="57"/>
+      <c r="BE1" s="57"/>
+      <c r="BF1" s="57"/>
+      <c r="BG1" s="57"/>
+      <c r="BH1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="BI1" s="58"/>
-      <c r="BJ1" s="59"/>
+      <c r="BI1" s="59"/>
+      <c r="BJ1" s="60"/>
     </row>
     <row r="2" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="55" t="s">
         <v>197</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2609,7 +2613,9 @@
       <c r="J6" s="16">
         <v>1100</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="55" t="s">
+        <v>198</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" s="9"/>
       <c r="N6" s="17"/>
@@ -33878,7 +33884,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -33892,19 +33898,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="59"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="60"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -36407,10 +36413,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="60"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
umbaran frigate bug fixes&combat power recalculation
</commit_message>
<xml_diff>
--- a/modding resources/Stats_Calc.xlsx
+++ b/modding resources/Stats_Calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFOLDER\IanLee\FOTR Submodding assests\FotR_Enhanced\modding resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D946B4D5-EDA5-48C4-93C2-E9885FF9821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854464F6-4399-4298-8D9C-2988D376EFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,7 +781,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="200">
   <si>
     <t>Unit</t>
   </si>
@@ -1042,9 +1042,6 @@
   </si>
   <si>
     <t>Light Rapid Laser</t>
-  </si>
-  <si>
-    <t>Dual Light Rapid Laser</t>
   </si>
   <si>
     <t>Quad Light Rapid Laser</t>
@@ -1384,6 +1381,14 @@
     <t>ArmourG_</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>ArmourS_Frigate</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dual Light Rapid Laser</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1584,7 +1589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1752,6 +1757,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1975,10 +1986,10 @@
   <dimension ref="A1:BJ1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AX3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="BF3" sqref="BF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2092,7 +2103,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -2460,7 +2471,7 @@
     </row>
     <row r="4" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -2526,7 +2537,7 @@
     </row>
     <row r="5" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
@@ -2536,32 +2547,85 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>1300</v>
+      </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
+      <c r="H5" s="3">
+        <v>19.25</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="16">
+        <v>1200</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="L5" s="3">
+        <v>170</v>
+      </c>
+      <c r="M5" s="9">
+        <v>-1</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="3">
+        <v>4</v>
+      </c>
+      <c r="P5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <v>2550</v>
+      </c>
+      <c r="S5" s="18">
+        <f>IFERROR((VLOOKUP(N5,Projectiles!$A:$D,4,FALSE)*O5*P5)/(Q5 + IF(P5 &gt; 1, P3*0.2, 0)),0)</f>
+        <v>62.857142857142861</v>
+      </c>
+      <c r="T5" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="U5" s="9">
+        <v>4</v>
+      </c>
+      <c r="V5" s="3">
+        <v>2</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="X5" s="3">
+        <v>1850</v>
+      </c>
+      <c r="Y5" s="5">
+        <f>IFERROR((VLOOKUP(T5,Projectiles!$A:$D,4,FALSE)*U5*V5)/(W5 + IF(V5 &gt; 1, V5*0.2, 0)),0)</f>
+        <v>10</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA5" s="12">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>1.7</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>1600</v>
+      </c>
+      <c r="AE5" s="5">
+        <f>IFERROR((VLOOKUP(Z5,Projectiles!$A:$D,4,FALSE)*AA5*AB5)/(AC5 + IF(AB5 &gt; 1, AB5*0.2, 0)),0)</f>
+        <v>14.285714285714285</v>
+      </c>
       <c r="AF5" s="4"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
@@ -2580,15 +2644,39 @@
       <c r="AU5" s="3"/>
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
-      <c r="AX5" s="6"/>
-      <c r="AY5" s="7"/>
-      <c r="AZ5" s="7"/>
-      <c r="BA5" s="7"/>
-      <c r="BB5" s="7"/>
-      <c r="BC5" s="8"/>
-      <c r="BD5" s="7"/>
-      <c r="BE5" s="7"/>
-      <c r="BF5" s="7"/>
+      <c r="AX5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="7">
+        <v>11</v>
+      </c>
+      <c r="BA5" s="7">
+        <f>SUM(S5,Y5,AE5,AK5,AQ5,AW5)</f>
+        <v>87.142857142857139</v>
+      </c>
+      <c r="BB5" s="7">
+        <f>BA5*(1+(0.05*M5))</f>
+        <v>82.785714285714278</v>
+      </c>
+      <c r="BC5" s="8">
+        <f>FLOOR(SQRT((1.5*BB5)*SUM((F5 + 1000 * H5/3) * VLOOKUP(I5, 'DamageArmour Matrices'!$J$2:$K$9,2,FALSE),J5 * VLOOKUP(K5, 'DamageArmour Matrices'!$H$2:$I$9,2,FALSE))),1)</f>
+        <v>612</v>
+      </c>
+      <c r="BD5" s="7">
+        <f>BC5/C5</f>
+        <v>0.51</v>
+      </c>
+      <c r="BE5" s="68">
+        <f>BC5/B5</f>
+        <v>122.4</v>
+      </c>
+      <c r="BF5" s="68">
+        <f>BA5/B5</f>
+        <v>17.428571428571427</v>
+      </c>
       <c r="BG5" s="5"/>
       <c r="BH5" s="3"/>
       <c r="BI5" s="3"/>
@@ -2596,7 +2684,7 @@
     </row>
     <row r="6" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -2614,7 +2702,7 @@
         <v>1100</v>
       </c>
       <c r="K6" s="55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="9"/>
@@ -20037,7 +20125,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31583,7 +31671,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31688,8 +31776,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>87</v>
+      <c r="A6" s="67" t="s">
+        <v>199</v>
       </c>
       <c r="B6" s="3">
         <f>B5*2</f>
@@ -31708,7 +31796,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="3">
         <f>B5*4</f>
@@ -31727,7 +31815,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -31745,7 +31833,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="3">
         <f>B8*2</f>
@@ -31764,7 +31852,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="3">
         <f>B8*4</f>
@@ -31783,7 +31871,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="3">
         <v>1.5</v>
@@ -31801,7 +31889,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="3">
         <f>B11*2</f>
@@ -31820,7 +31908,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="3">
         <f>B11*4</f>
@@ -31839,7 +31927,7 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -31857,7 +31945,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3">
         <f>B14*2</f>
@@ -31876,7 +31964,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="3">
         <f>B14*4</f>
@@ -31895,7 +31983,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -31913,7 +32001,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="3">
         <f>B17*2</f>
@@ -31932,7 +32020,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="3">
         <f>B17*4</f>
@@ -31957,7 +32045,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="3">
         <f>((VLOOKUP(C20, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B20)+(VLOOKUP(C20, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B20))/2</f>
@@ -31969,14 +32057,14 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="3">
         <f>B20*2</f>
         <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="3">
         <f>((VLOOKUP(C21, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B21)+(VLOOKUP(C21, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B21))/2</f>
@@ -31988,14 +32076,14 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="3">
         <f>B20*3</f>
         <v>60</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="3">
         <f>((VLOOKUP(C22, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B22)+(VLOOKUP(C22, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B22))/2</f>
@@ -32007,14 +32095,14 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="3">
         <f>B20*4</f>
         <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="3">
         <f>((VLOOKUP(C23, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B23)+(VLOOKUP(C23, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B23))/2</f>
@@ -32026,14 +32114,14 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" s="3">
         <f>B20*8</f>
         <v>160</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" s="3">
         <f>((VLOOKUP(C24, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B24)+(VLOOKUP(C24, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B24))/2</f>
@@ -32045,13 +32133,13 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="3">
         <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="3">
         <f>((VLOOKUP(C25, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B25)+(VLOOKUP(C25, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B25))/2</f>
@@ -32063,14 +32151,14 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" s="3">
         <f>B25*2</f>
         <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="3">
         <f>((VLOOKUP(C26, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B26)+(VLOOKUP(C26, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B26))/2</f>
@@ -32082,14 +32170,14 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="3">
         <f>B25*3</f>
         <v>90</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="3">
         <f>((VLOOKUP(C27, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B27)+(VLOOKUP(C27, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B27))/2</f>
@@ -32101,14 +32189,14 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="3">
         <f>B25*4</f>
         <v>120</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28" s="3">
         <f>((VLOOKUP(C28, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B28)+(VLOOKUP(C28, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B28))/2</f>
@@ -32120,14 +32208,14 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="3">
         <f>B25*8</f>
         <v>240</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" s="3">
         <f>((VLOOKUP(C29, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B29)+(VLOOKUP(C29, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B29))/2</f>
@@ -32139,13 +32227,13 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="3">
         <v>40</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="3">
         <f>((VLOOKUP(C30, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B30)+(VLOOKUP(C30, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B30))/2</f>
@@ -32157,14 +32245,14 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="3">
         <f>B30*2</f>
         <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="3">
         <f>((VLOOKUP(C31, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B31)+(VLOOKUP(C31, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B31))/2</f>
@@ -32176,14 +32264,14 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="3">
         <f>B30*3</f>
         <v>120</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D32" s="3">
         <f>((VLOOKUP(C32, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B32)+(VLOOKUP(C32, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B32))/2</f>
@@ -32195,14 +32283,14 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B33" s="3">
         <f>B30*4</f>
         <v>160</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" s="3">
         <f>((VLOOKUP(C33, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B33)+(VLOOKUP(C33, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B33))/2</f>
@@ -32214,14 +32302,14 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B34" s="3">
         <f>B30*8</f>
         <v>320</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" s="3">
         <f>((VLOOKUP(C34, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B34)+(VLOOKUP(C34, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B34))/2</f>
@@ -32233,13 +32321,13 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" s="3">
         <v>100</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" s="3">
         <f>((VLOOKUP(C35, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B35)+(VLOOKUP(C35, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B35))/2</f>
@@ -32251,13 +32339,13 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" s="3">
         <v>2500</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" s="3">
         <f>((VLOOKUP(C36, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B36)+(VLOOKUP(C36, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B36))/2</f>
@@ -32275,7 +32363,7 @@
         <v>15</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="3">
         <f>((VLOOKUP(C37, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B37)+(VLOOKUP(C37, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B37))/2</f>
@@ -32287,14 +32375,14 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="3">
         <f>B37*2</f>
         <v>30</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="3">
         <f>((VLOOKUP(C38, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B38)+(VLOOKUP(C38, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B38))/2</f>
@@ -32306,14 +32394,14 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="3">
         <f>B37*3</f>
         <v>45</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" s="3">
         <f>((VLOOKUP(C39, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B39)+(VLOOKUP(C39, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B39))/2</f>
@@ -32325,14 +32413,14 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B40" s="3">
         <f>B37*4</f>
         <v>60</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="3">
         <f>((VLOOKUP(C40, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B40)+(VLOOKUP(C40, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B40))/2</f>
@@ -32344,14 +32432,14 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B41" s="3">
         <f>B37*8</f>
         <v>120</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D41" s="3">
         <f>((VLOOKUP(C41, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B41)+(VLOOKUP(C41, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B41))/2</f>
@@ -32363,13 +32451,13 @@
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B42" s="3">
         <v>22.5</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42" s="3">
         <f>((VLOOKUP(C42, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B42)+(VLOOKUP(C42, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B42))/2</f>
@@ -32381,14 +32469,14 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" s="3">
         <f>B42*2</f>
         <v>45</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" s="3">
         <f>((VLOOKUP(C43, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B43)+(VLOOKUP(C43, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B43))/2</f>
@@ -32400,14 +32488,14 @@
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B44" s="3">
         <f>B42*3</f>
         <v>67.5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D44" s="3">
         <f>((VLOOKUP(C44, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B44)+(VLOOKUP(C44, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B44))/2</f>
@@ -32419,14 +32507,14 @@
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" s="3">
         <f>B42*4</f>
         <v>90</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="3">
         <f>((VLOOKUP(C45, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B45)+(VLOOKUP(C45, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B45))/2</f>
@@ -32438,14 +32526,14 @@
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B46" s="3">
         <f>B42*8</f>
         <v>180</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D46" s="3">
         <f>((VLOOKUP(C46, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B46)+(VLOOKUP(C46, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B46))/2</f>
@@ -32457,13 +32545,13 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B47" s="3">
         <v>30</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D47" s="3">
         <f>((VLOOKUP(C47, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B47)+(VLOOKUP(C47, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B47))/2</f>
@@ -32475,14 +32563,14 @@
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B48" s="3">
         <f>B47*2</f>
         <v>60</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="3">
         <f>((VLOOKUP(C48, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B48)+(VLOOKUP(C48, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B48))/2</f>
@@ -32494,14 +32582,14 @@
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B49" s="3">
         <f>B47*3</f>
         <v>90</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49" s="3">
         <f>((VLOOKUP(C49, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B49)+(VLOOKUP(C49, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B49))/2</f>
@@ -32513,14 +32601,14 @@
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B50" s="3">
         <f>B47*4</f>
         <v>120</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50" s="3">
         <f>((VLOOKUP(C50, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B50)+(VLOOKUP(C50, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B50))/2</f>
@@ -32532,14 +32620,14 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B51" s="3">
         <f>B47*8</f>
         <v>240</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D51" s="3">
         <f>((VLOOKUP(C51, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B51)+(VLOOKUP(C51, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B51))/2</f>
@@ -32551,13 +32639,13 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B52" s="3">
         <v>75</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D52" s="3">
         <f>((VLOOKUP(C52, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B52)+(VLOOKUP(C52, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B52))/2</f>
@@ -32569,13 +32657,13 @@
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" s="3">
         <v>2000</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D53" s="3">
         <f>((VLOOKUP(C53, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B53)+(VLOOKUP(C53, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B53))/2</f>
@@ -32587,13 +32675,13 @@
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B54" s="3">
         <v>6</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D54" s="3">
         <f>((VLOOKUP(C54, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B54)+(VLOOKUP(C54, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B54))/2</f>
@@ -32605,13 +32693,13 @@
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="3">
         <v>18</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D55" s="3">
         <f>((VLOOKUP(C55, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B55)+(VLOOKUP(C55, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B55))/2</f>
@@ -32623,13 +32711,13 @@
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B56" s="3">
         <v>54</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D56" s="3">
         <f>((VLOOKUP(C56, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B56)+(VLOOKUP(C56, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B56))/2</f>
@@ -32641,13 +32729,13 @@
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B57" s="3">
         <v>24</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D57" s="3">
         <f>((VLOOKUP(C57, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B57)+(VLOOKUP(C57, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B57))/2</f>
@@ -32659,13 +32747,13 @@
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B58" s="3">
         <v>72</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D58" s="3">
         <f>((VLOOKUP(C58, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B58)+(VLOOKUP(C58, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B58))/2</f>
@@ -32677,13 +32765,13 @@
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B59" s="16">
         <v>18</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" s="3">
         <f>((VLOOKUP(C59, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B59)+(VLOOKUP(C59, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B59))/2</f>
@@ -32695,13 +32783,13 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B60" s="9">
         <v>3</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D60" s="3">
         <f>((VLOOKUP(C60, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B60)+(VLOOKUP(C60, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B60))/2</f>
@@ -32713,7 +32801,7 @@
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B61" s="43"/>
       <c r="C61" s="43"/>
@@ -32738,7 +32826,7 @@
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B63" s="3">
         <v>0.75</v>
@@ -32754,13 +32842,13 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B64" s="3">
         <v>2</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D64" s="3">
         <f>((VLOOKUP(C64, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B64)+(VLOOKUP(C64, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B64))/2</f>
@@ -32770,13 +32858,13 @@
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B65" s="3">
         <v>2</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D65" s="3">
         <f>((VLOOKUP(C65, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B65)+(VLOOKUP(C65, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B65))/2</f>
@@ -32792,7 +32880,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D66" s="3">
         <f>((VLOOKUP(C66, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B66)+(VLOOKUP(C66, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B66))/2</f>
@@ -32802,13 +32890,13 @@
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B67" s="3">
         <v>20</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D67" s="3">
         <f>((VLOOKUP(C67, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B67)+(VLOOKUP(C67, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B67))/2</f>
@@ -32818,13 +32906,13 @@
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B68" s="3">
         <v>20</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D68" s="3">
         <f>((VLOOKUP(C68, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B68)+(VLOOKUP(C68, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B68))/2</f>
@@ -32840,7 +32928,7 @@
         <v>40</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D69" s="3">
         <f>((VLOOKUP(C69, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B69)+(VLOOKUP(C69, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B69))/2</f>
@@ -32850,13 +32938,13 @@
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B70" s="3">
         <v>17</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D70" s="3">
         <f>((VLOOKUP(C70, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B70)+(VLOOKUP(C70, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B70))/2</f>
@@ -32872,7 +32960,7 @@
         <v>34</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D71" s="3">
         <f>((VLOOKUP(C71, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B71)+(VLOOKUP(C71, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B71))/2</f>
@@ -32882,13 +32970,13 @@
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B72" s="3">
         <v>10</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D72" s="3">
         <f>((VLOOKUP(C72, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B72)+(VLOOKUP(C72, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B72))/2</f>
@@ -32898,13 +32986,13 @@
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B73" s="3">
         <v>17</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D73" s="3">
         <f>((VLOOKUP(C73, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B73)+(VLOOKUP(C73, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B73))/2</f>
@@ -32914,13 +33002,13 @@
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B74" s="3">
         <v>8</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D74" s="3">
         <f>((VLOOKUP(C74, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B74)+(VLOOKUP(C74, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B74))/2</f>
@@ -32930,13 +33018,13 @@
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B75" s="46">
         <v>0.5</v>
       </c>
       <c r="C75" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D75" s="47">
         <f>((VLOOKUP(C75, 'DamageArmour Matrices'!$A$1:$E$66,3,FALSE)*B75)+(VLOOKUP(C75, 'DamageArmour Matrices'!$A$1:$E$66,5,FALSE)*B75))/2</f>
@@ -33899,7 +33987,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -33917,44 +34005,44 @@
         <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -33962,7 +34050,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I9" si="0">1-AVERAGE(C3,C11,C27,C35,C43)</f>
@@ -33980,13 +34068,13 @@
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="3">
         <v>0.85</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -33994,7 +34082,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="0"/>
@@ -34012,13 +34100,13 @@
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="3">
         <v>0.625</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E5" s="3">
         <v>0.75</v>
@@ -34026,7 +34114,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="0"/>
@@ -34044,13 +34132,13 @@
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" s="3">
         <v>0.5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E6" s="3">
         <v>0.5</v>
@@ -34076,13 +34164,13 @@
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" s="3">
         <v>0.25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E7" s="3">
         <v>0.5</v>
@@ -34090,7 +34178,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="0"/>
@@ -34108,13 +34196,13 @@
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C8" s="3">
         <v>0.1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="3">
         <v>0.25</v>
@@ -34122,7 +34210,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="0"/>
@@ -34140,13 +34228,13 @@
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C9" s="3">
         <v>0.1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" s="3">
         <v>0.25</v>
@@ -34154,7 +34242,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="0"/>
@@ -34174,21 +34262,21 @@
         <v>83</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="50">
         <f>MEDIAN(C3:C9)</f>
         <v>0.5</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" s="50">
         <f>MEDIAN(E3:E9)</f>
         <v>0.5</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G10" s="50">
         <f>(C10+E10)/2</f>
@@ -34201,16 +34289,16 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E11" s="3">
         <v>0.75</v>
@@ -34225,13 +34313,13 @@
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="3">
         <v>0.8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" s="3">
         <v>0.75</v>
@@ -34246,13 +34334,13 @@
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="3">
         <v>0.7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E13" s="3">
         <v>0.75</v>
@@ -34267,13 +34355,13 @@
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="3">
         <v>0.6</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E14" s="3">
         <v>0.5</v>
@@ -34288,13 +34376,13 @@
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="3">
         <v>0.5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E15" s="3">
         <v>0.5</v>
@@ -34309,13 +34397,13 @@
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C16" s="3">
         <v>0.5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E16" s="3">
         <v>0.25</v>
@@ -34330,13 +34418,13 @@
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C17" s="3">
         <v>0.25</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E17" s="3">
         <v>0.25</v>
@@ -34350,24 +34438,24 @@
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="50">
         <f>MEDIAN(C11:C17)</f>
         <v>0.6</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E18" s="50">
         <f>MEDIAN(E11:E17)</f>
         <v>0.5</v>
       </c>
       <c r="F18" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G18" s="50">
         <f>(C18+E18)/2</f>
@@ -34380,16 +34468,16 @@
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -34404,13 +34492,13 @@
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -34425,13 +34513,13 @@
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -34446,13 +34534,13 @@
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -34467,13 +34555,13 @@
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -34488,13 +34576,13 @@
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -34509,13 +34597,13 @@
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -34529,24 +34617,24 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C26" s="50">
         <f>MEDIAN(C19:C25)</f>
         <v>0</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E26" s="50">
         <f>MEDIAN(E19:E25)</f>
         <v>1</v>
       </c>
       <c r="F26" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G26" s="50">
         <f>(C26+E26)/2</f>
@@ -34559,16 +34647,16 @@
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" s="3">
         <v>0.75</v>
@@ -34583,13 +34671,13 @@
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E28" s="3">
         <v>0.75</v>
@@ -34604,13 +34692,13 @@
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E29" s="3">
         <v>0.75</v>
@@ -34625,13 +34713,13 @@
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E30" s="3">
         <v>0.5</v>
@@ -34646,13 +34734,13 @@
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31" s="3">
         <v>0.75</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E31" s="3">
         <v>0.5</v>
@@ -34667,13 +34755,13 @@
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C32" s="3">
         <v>0.625</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E32" s="3">
         <v>0.5</v>
@@ -34688,13 +34776,13 @@
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C33" s="3">
         <v>0.75</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E33" s="3">
         <v>0.5</v>
@@ -34708,24 +34796,24 @@
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C34" s="50">
         <f>MEDIAN(C27:C33)</f>
         <v>1</v>
       </c>
       <c r="D34" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E34" s="50">
         <f>MEDIAN(E27:E33)</f>
         <v>0.5</v>
       </c>
       <c r="F34" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G34" s="50">
         <f>(C34+E34)/2</f>
@@ -34738,16 +34826,16 @@
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
@@ -34762,13 +34850,13 @@
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C36" s="3">
         <v>0.9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E36" s="3">
         <v>1</v>
@@ -34783,13 +34871,13 @@
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C37" s="3">
         <v>0.9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -34804,13 +34892,13 @@
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" s="3">
         <v>0.8</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -34825,13 +34913,13 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C39" s="3">
         <v>0.8</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
@@ -34846,13 +34934,13 @@
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C40" s="3">
         <v>0.75</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E40" s="3">
         <v>1</v>
@@ -34867,13 +34955,13 @@
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C41" s="3">
         <v>0.75</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E41" s="3">
         <v>1</v>
@@ -34887,24 +34975,24 @@
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C42" s="50">
         <f>MEDIAN(C35:C41)</f>
         <v>0.8</v>
       </c>
       <c r="D42" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E42" s="50">
         <f>MEDIAN(E35:E41)</f>
         <v>1</v>
       </c>
       <c r="F42" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G42" s="50">
         <f>(C42+E42)/2</f>
@@ -34917,16 +35005,16 @@
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E43" s="3">
         <v>1</v>
@@ -34941,13 +35029,13 @@
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C44" s="3">
         <v>0.75</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E44" s="3">
         <v>0.75</v>
@@ -34962,13 +35050,13 @@
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C45" s="3">
         <v>0.5</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E45" s="3">
         <v>0.5</v>
@@ -34983,13 +35071,13 @@
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C46" s="3">
         <v>0.25</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E46" s="3">
         <v>0.5</v>
@@ -35004,13 +35092,13 @@
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C47" s="3">
         <v>0.25</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E47" s="3">
         <v>0.5</v>
@@ -35025,13 +35113,13 @@
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C48" s="3">
         <v>0.125</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E48" s="3">
         <v>0.25</v>
@@ -35046,13 +35134,13 @@
     <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C49" s="3">
         <v>0.125</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E49" s="3">
         <v>0.25</v>
@@ -35066,24 +35154,24 @@
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C50" s="50">
         <f>MEDIAN(C43:C49)</f>
         <v>0.25</v>
       </c>
       <c r="D50" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E50" s="50">
         <f>MEDIAN(E43:E49)</f>
         <v>0.5</v>
       </c>
       <c r="F50" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G50" s="50">
         <f>(C50+E50)/2</f>
@@ -35096,16 +35184,16 @@
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C51" s="3">
         <v>0</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E51" s="3">
         <v>1</v>
@@ -35120,13 +35208,13 @@
     <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C52" s="3">
         <v>0</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
@@ -35141,13 +35229,13 @@
     <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C53" s="3">
         <v>0</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -35162,13 +35250,13 @@
     <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C54" s="3">
         <v>0</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E54" s="3">
         <v>0.75</v>
@@ -35183,13 +35271,13 @@
     <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C55" s="3">
         <v>0</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E55" s="3">
         <v>0.75</v>
@@ -35204,13 +35292,13 @@
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C56" s="3">
         <v>0</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E56" s="3">
         <v>0.5</v>
@@ -35225,13 +35313,13 @@
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C57" s="3">
         <v>0</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E57" s="3">
         <v>0.5</v>
@@ -35245,24 +35333,24 @@
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C58" s="50">
         <f>MEDIAN(C51:C57)</f>
         <v>0</v>
       </c>
       <c r="D58" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E58" s="50">
         <f>MEDIAN(E51:E57)</f>
         <v>0.75</v>
       </c>
       <c r="F58" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G58" s="50">
         <f>(C58+E58)/2</f>
@@ -35275,16 +35363,16 @@
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C59" s="3">
         <v>0</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E59" s="3">
         <v>0</v>
@@ -35299,13 +35387,13 @@
     <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C60" s="3">
         <v>1</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E60" s="3">
         <v>0.75</v>
@@ -35320,13 +35408,13 @@
     <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C61" s="3">
         <v>1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E61" s="3">
         <v>0.75</v>
@@ -35341,13 +35429,13 @@
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C62" s="3">
         <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E62" s="3">
         <v>0.75</v>
@@ -35362,13 +35450,13 @@
     <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C63" s="3">
         <v>1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E63" s="3">
         <v>0.75</v>
@@ -35383,13 +35471,13 @@
     <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E64" s="3">
         <v>0.75</v>
@@ -35404,13 +35492,13 @@
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C65" s="3">
         <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E65" s="3">
         <v>0.75</v>
@@ -35424,24 +35512,24 @@
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B66" s="52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C66" s="52">
         <f>MEDIAN(C59:C65)</f>
         <v>1</v>
       </c>
       <c r="D66" s="52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E66" s="52">
         <f>MEDIAN(E59:E65)</f>
         <v>0.75</v>
       </c>
       <c r="F66" s="52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G66" s="52">
         <f>(C66+E66)/2</f>
@@ -36404,7 +36492,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -36414,13 +36502,13 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="60"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" s="5">
         <v>0.25</v>
@@ -36428,7 +36516,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="5">
         <v>0.5</v>
@@ -36436,7 +36524,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="5">
         <v>0.75</v>
@@ -36444,7 +36532,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -36460,7 +36548,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7" s="5">
         <v>1.5</v>
@@ -36468,7 +36556,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="5">
         <v>1.75</v>
@@ -36476,7 +36564,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9" s="5">
         <v>2</v>
@@ -36484,7 +36572,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10" s="5">
         <v>2.25</v>
@@ -36492,7 +36580,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" s="48">
         <v>2.5</v>

</xml_diff>